<commit_message>
Actualizar documentación y notebooks de exploración
- Agregar nota sobre calidad de datos de violencia en methodology.md
- Actualizar logo en notebook idb-stats.ipynb
- Actualizar estadísticas en tabla idb_stats.xlsx
- Ajustar permisos de archivos del proyecto
</commit_message>
<xml_diff>
--- a/outputs/tables/old_idb_stats/idb_stats.xlsx
+++ b/outputs/tables/old_idb_stats/idb_stats.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/jd_heredian_uniandes_edu_co/Documents/early-warning-atypical-violence-forecast/outputs/tables/old_idb_stats/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_9FA744B291E6E8BF891C87CE7A2F596721B12B33" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B817364C-A854-CF4D-A5AA-8EF5B7C17794}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -31,12 +37,6 @@
     <t>Maximum</t>
   </si>
   <si>
-    <t>Proportion of Atypical Homicide Municipal Quarters (std)</t>
-  </si>
-  <si>
-    <t>Proportion of Atypical Homicide Municipal Quarters (2x std)</t>
-  </si>
-  <si>
     <t>Terrorism</t>
   </si>
   <si>
@@ -53,13 +53,19 @@
   </si>
   <si>
     <t>CVAI</t>
+  </si>
+  <si>
+    <t>Proportion of Atypical Violence Municipal Quarters (2x std)</t>
+  </si>
+  <si>
+    <t>Proportion of Atypical Violence Municipal Quarters (std)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,10 +117,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -122,13 +140,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -166,7 +192,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -200,6 +226,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -234,9 +261,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -409,190 +437,200 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="A1:H7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="6" width="8.83203125" style="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:8" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B2" s="5">
+        <v>2687</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2.1</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5">
+        <v>29</v>
+      </c>
+      <c r="G2" s="5">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="H2" s="5">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B3" s="5">
+        <v>24890</v>
+      </c>
+      <c r="C3" s="5">
+        <v>4.7</v>
+      </c>
+      <c r="D3" s="5">
+        <v>18.3</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5">
+        <v>729</v>
+      </c>
+      <c r="G3" s="5">
+        <v>21.88</v>
+      </c>
+      <c r="H3" s="5">
+        <v>11.84</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>2687</v>
-      </c>
-      <c r="C2">
-        <v>2.2</v>
-      </c>
-      <c r="D2">
-        <v>2.1</v>
-      </c>
-      <c r="E2">
+      <c r="B4" s="5">
+        <v>47997</v>
+      </c>
+      <c r="C4" s="5">
+        <v>6.7</v>
+      </c>
+      <c r="D4" s="5">
+        <v>24.8</v>
+      </c>
+      <c r="E4" s="5">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>29</v>
-      </c>
-      <c r="G2">
-        <v>17.4</v>
-      </c>
-      <c r="H2">
-        <v>8.75</v>
+      <c r="F4" s="5">
+        <v>614</v>
+      </c>
+      <c r="G4" s="5">
+        <v>17.98</v>
+      </c>
+      <c r="H4" s="5">
+        <v>8.5299999999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>24890</v>
-      </c>
-      <c r="C3">
-        <v>4.7</v>
-      </c>
-      <c r="D3">
-        <v>18.3</v>
-      </c>
-      <c r="E3">
+      <c r="B5" s="5">
+        <v>259</v>
+      </c>
+      <c r="C5" s="5">
+        <v>3.8</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1.9</v>
+      </c>
+      <c r="E5" s="5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="5">
+        <v>18</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5">
+        <v>10538</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2.7</v>
+      </c>
+      <c r="D6" s="5">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E6" s="5">
         <v>1</v>
       </c>
-      <c r="F3">
-        <v>729</v>
-      </c>
-      <c r="G3">
-        <v>21.88</v>
-      </c>
-      <c r="H3">
-        <v>11.84</v>
+      <c r="F6" s="5">
+        <v>179</v>
+      </c>
+      <c r="G6" s="5">
+        <v>14.46</v>
+      </c>
+      <c r="H6" s="5">
+        <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>47997</v>
-      </c>
-      <c r="C4">
-        <v>6.7</v>
-      </c>
-      <c r="D4">
-        <v>24.8</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>614</v>
-      </c>
-      <c r="G4">
-        <v>17.98</v>
-      </c>
-      <c r="H4">
-        <v>8.529999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
-        <v>259</v>
-      </c>
-      <c r="C5">
-        <v>3.8</v>
-      </c>
-      <c r="D5">
-        <v>1.9</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>18</v>
-      </c>
-      <c r="G5">
+      <c r="B7" s="5">
+        <v>67273</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="D7" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E7" s="5">
         <v>0</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>10538</v>
-      </c>
-      <c r="C6">
-        <v>2.7</v>
-      </c>
-      <c r="D6">
-        <v>4.6</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>179</v>
-      </c>
-      <c r="G6">
-        <v>14.46</v>
-      </c>
-      <c r="H6">
-        <v>8.050000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>67273</v>
-      </c>
-      <c r="C7">
-        <v>1.4</v>
-      </c>
-      <c r="D7">
-        <v>2.2</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
+      <c r="F7" s="5">
         <v>53.5</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="5">
         <v>17.05</v>
       </c>
-      <c r="H7">
-        <v>8.619999999999999</v>
+      <c r="H7" s="5">
+        <v>8.6199999999999992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reorganizar notebooks de exploración y actualizar estadísticas IDB
- Renombrar notebook de replicación y actualizar encabezado
- Reorganizar notebook idb-stats con nuevo nombre (-1_idb-stats.ipynb)
- Agregar estadísticas de IGC e IA (índices JEP) a la tabla
- Cambiar nombre de CVAI a IACV para consistencia
- Actualizar archivo idb_stats.xlsx con nuevas métricas
</commit_message>
<xml_diff>
--- a/outputs/tables/old_idb_stats/idb_stats.xlsx
+++ b/outputs/tables/old_idb_stats/idb_stats.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/jd_heredian_uniandes_edu_co/Documents/early-warning-atypical-violence-forecast/outputs/tables/old_idb_stats/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_9FA744B291E6E8BF891C87CE7A2F596721B12B33" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B817364C-A854-CF4D-A5AA-8EF5B7C17794}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Number of Observations</t>
   </si>
@@ -37,6 +31,12 @@
     <t>Maximum</t>
   </si>
   <si>
+    <t>Proportion of Atypical Homicide Municipal Quarters (std)</t>
+  </si>
+  <si>
+    <t>Proportion of Atypical Homicide Municipal Quarters (2x std)</t>
+  </si>
+  <si>
     <t>Terrorism</t>
   </si>
   <si>
@@ -55,17 +55,17 @@
     <t>CVAI</t>
   </si>
   <si>
-    <t>Proportion of Atypical Violence Municipal Quarters (2x std)</t>
-  </si>
-  <si>
-    <t>Proportion of Atypical Violence Municipal Quarters (std)</t>
+    <t>IGC</t>
+  </si>
+  <si>
+    <t>IA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,22 +117,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -140,21 +128,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -192,7 +172,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -226,7 +206,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -261,10 +240,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -437,200 +415,230 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="A1:H7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="6" width="8.83203125" style="1"/>
-    <col min="7" max="7" width="15.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16" style="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="61" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:8">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>2687</v>
+      </c>
+      <c r="C2">
+        <v>2.2</v>
+      </c>
+      <c r="D2">
+        <v>2.1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>29</v>
+      </c>
+      <c r="G2">
+        <v>17.4</v>
+      </c>
+      <c r="H2">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>24890</v>
+      </c>
+      <c r="C3">
+        <v>4.7</v>
+      </c>
+      <c r="D3">
+        <v>18.3</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>729</v>
+      </c>
+      <c r="G3">
+        <v>21.88</v>
+      </c>
+      <c r="H3">
+        <v>11.84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>47997</v>
+      </c>
+      <c r="C4">
+        <v>6.7</v>
+      </c>
+      <c r="D4">
+        <v>24.8</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>614</v>
+      </c>
+      <c r="G4">
+        <v>17.98</v>
+      </c>
+      <c r="H4">
+        <v>8.529999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>259</v>
+      </c>
+      <c r="C5">
+        <v>3.8</v>
+      </c>
+      <c r="D5">
+        <v>1.9</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>18</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>10538</v>
+      </c>
+      <c r="C6">
+        <v>2.7</v>
+      </c>
+      <c r="D6">
+        <v>4.6</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>179</v>
+      </c>
+      <c r="G6">
+        <v>14.46</v>
+      </c>
+      <c r="H6">
+        <v>8.050000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5">
-        <v>2687</v>
-      </c>
-      <c r="C2" s="5">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D2" s="5">
-        <v>2.1</v>
-      </c>
-      <c r="E2" s="5">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5">
-        <v>29</v>
-      </c>
-      <c r="G2" s="5">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="H2" s="5">
-        <v>8.75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="5">
-        <v>24890</v>
-      </c>
-      <c r="C3" s="5">
-        <v>4.7</v>
-      </c>
-      <c r="D3" s="5">
-        <v>18.3</v>
-      </c>
-      <c r="E3" s="5">
-        <v>1</v>
-      </c>
-      <c r="F3" s="5">
-        <v>729</v>
-      </c>
-      <c r="G3" s="5">
-        <v>21.88</v>
-      </c>
-      <c r="H3" s="5">
-        <v>11.84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5">
-        <v>47997</v>
-      </c>
-      <c r="C4" s="5">
-        <v>6.7</v>
-      </c>
-      <c r="D4" s="5">
-        <v>24.8</v>
-      </c>
-      <c r="E4" s="5">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5">
-        <v>614</v>
-      </c>
-      <c r="G4" s="5">
-        <v>17.98</v>
-      </c>
-      <c r="H4" s="5">
-        <v>8.5299999999999994</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="5">
-        <v>259</v>
-      </c>
-      <c r="C5" s="5">
-        <v>3.8</v>
-      </c>
-      <c r="D5" s="5">
-        <v>1.9</v>
-      </c>
-      <c r="E5" s="5">
-        <v>3</v>
-      </c>
-      <c r="F5" s="5">
-        <v>18</v>
-      </c>
-      <c r="G5" s="5">
+      <c r="B7">
+        <v>67273</v>
+      </c>
+      <c r="C7">
+        <v>1.4</v>
+      </c>
+      <c r="D7">
+        <v>2.2</v>
+      </c>
+      <c r="E7">
         <v>0</v>
       </c>
-      <c r="H5" s="5">
+      <c r="F7">
+        <v>53.5</v>
+      </c>
+      <c r="G7">
+        <v>17.05</v>
+      </c>
+      <c r="H7">
+        <v>8.619999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>26920</v>
+      </c>
+      <c r="C8">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5">
-        <v>10538</v>
-      </c>
-      <c r="C6" s="5">
-        <v>2.7</v>
-      </c>
-      <c r="D6" s="5">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E6" s="5">
-        <v>1</v>
-      </c>
-      <c r="F6" s="5">
-        <v>179</v>
-      </c>
-      <c r="G6" s="5">
-        <v>14.46</v>
-      </c>
-      <c r="H6" s="5">
-        <v>8.0500000000000007</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="D8">
+        <v>0.3</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>10</v>
       </c>
-      <c r="B7" s="5">
-        <v>67273</v>
-      </c>
-      <c r="C7" s="5">
-        <v>1.4</v>
-      </c>
-      <c r="D7" s="5">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E7" s="5">
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>26920</v>
+      </c>
+      <c r="C9">
+        <v>0.2</v>
+      </c>
+      <c r="D9">
+        <v>1.1</v>
+      </c>
+      <c r="E9">
         <v>0</v>
       </c>
-      <c r="F7" s="5">
-        <v>53.5</v>
-      </c>
-      <c r="G7" s="5">
-        <v>17.05</v>
-      </c>
-      <c r="H7" s="5">
-        <v>8.6199999999999992</v>
+      <c r="F9">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>